<commit_message>
Add new analysis and lod prefabs
</commit_message>
<xml_diff>
--- a/Cube Analisys.xlsx
+++ b/Cube Analisys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yre03/Dev/Saxion/TreeTerrainAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD946258-4413-3F46-836F-86A1B64D013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2116232B-1A43-6146-99A9-2926F38EBCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="5" xr2:uid="{2DB56CFA-1DDE-0E44-9320-4C6DD7670085}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="ExternalData_1" localSheetId="4" hidden="1">'regular cube again'!$A$1:$P$101</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'regular cube prefab'!$A$1:$P$101</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -10857,7 +10857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE952E87-A0C4-0C48-89F3-9DF55760A5E1}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -15943,7 +15943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28694523-CAC1-1C4B-A71B-744184DA8200}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView topLeftCell="B2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21027,7 +21027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5683292A-DB67-7E49-967E-87B02BC3D760}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -26113,7 +26113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1CB313-4DE9-B347-B91E-6AC75D5B2D87}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -36285,8 +36285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9802E6B9-44E7-4B4A-8F0E-EAF8F45088CF}">
   <dimension ref="B2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>